<commit_message>
update queue folder name
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thaibev\RPAOACTemplate\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E891F64-C294-438B-A95F-290147042755}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CA734C-4E57-4959-8301-46219F97C920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>Name</t>
   </si>
@@ -196,13 +196,46 @@
     <t>MailException</t>
   </si>
   <si>
-    <t>parnupon.k@thaibev.com</t>
-  </si>
-  <si>
     <t>\\10.7.54.107\sleaprpauna01\Thai Beverage Public Company Limited\OAC - RPA_Shared\{0}\process\{1}</t>
   </si>
   <si>
     <t>IsSapProcess</t>
+  </si>
+  <si>
+    <t>parnupong.k@thaibev.com</t>
+  </si>
+  <si>
+    <t>MaxConsecutiveSystemExceptions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of consecutive system exceptions allowed. If MaxConsecutiveSystemExceptions is reached, the job is stopped. To disable this feature, set the value to 0. </t>
+  </si>
+  <si>
+    <t>ExceptionMessage_ConsecutiveErrors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
+  </si>
+  <si>
+    <t>Error message in case MaxConsecutiveSystemExceptions number is reached.</t>
+  </si>
+  <si>
+    <t>RetryNumberGetTransactionItem</t>
+  </si>
+  <si>
+    <t>The number of times Get Transaction Item activity is retried in case of an exception. Must be an integer &gt;= 1.</t>
+  </si>
+  <si>
+    <t>RetryNumberSetTransactionStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of times Set transaction status activity is retried in case of an exception. Must be an integer &gt;= 1. </t>
+  </si>
+  <si>
+    <t>ShouldMarkJobAsFaulted</t>
+  </si>
+  <si>
+    <t>Must be TRUE or FALSE. If the value is TRUE and an error occurs in Initialization state or the MaxConsecutiveSystemExceptions is reached, the job is marked as Faulted.</t>
   </si>
 </sst>
 </file>
@@ -581,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -665,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>32</v>
@@ -716,7 +749,7 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="b">
         <v>1</v>
@@ -1719,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1765,114 +1798,174 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="14.4">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
       </c>
     </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>57</v>
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B19" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>